<commit_message>
freshed the planning sheet
</commit_message>
<xml_diff>
--- a/Team10Report.xlsx
+++ b/Team10Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klwj2\Desktop\study\Stevens\555\project 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yikanwang/Documents/Spring2021/SSW555/SSW-555-A-Project-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A81C71F-09D8-4B28-AF4B-22356D2B4695}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E2F735-DAE3-524B-8763-EDE43DD85B51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23055" yWindow="2250" windowWidth="28305" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -341,6 +341,18 @@
   </si>
   <si>
     <t>T029.02</t>
+  </si>
+  <si>
+    <t>Check marriage if before 14</t>
+  </si>
+  <si>
+    <t>check if marry twice at same time</t>
+  </si>
+  <si>
+    <t>WYK</t>
+  </si>
+  <si>
+    <t>coding</t>
   </si>
 </sst>
 </file>
@@ -351,7 +363,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,13 +727,13 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -749,7 +761,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -766,7 +778,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -783,7 +795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -794,7 +806,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
@@ -821,14 +833,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -845,7 +857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -862,7 +874,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -879,7 +891,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -896,7 +908,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -913,7 +925,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -930,7 +942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -947,7 +959,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -964,7 +976,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -996,14 +1008,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -1023,13 +1035,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>44259</v>
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="F3" s="6"/>
     </row>
@@ -1041,26 +1053,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7423B761-4644-4B14-9E93-F056AD5F843E}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="41.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="6" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="41.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="13" max="13" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.600000000000001" customHeight="1">
+    <row r="1" spans="1:13" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1089,7 +1101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1121,10 +1133,10 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1138,7 +1150,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -1152,7 +1164,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1164,10 +1176,10 @@
       </c>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1190,10 +1202,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1207,7 +1219,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -1218,7 +1230,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -1229,7 +1241,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1258,7 +1270,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1287,7 +1299,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>81</v>
       </c>
@@ -1316,7 +1328,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1345,7 +1357,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1374,7 +1386,7 @@
         <v>44258</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -1401,6 +1413,46 @@
       </c>
       <c r="I22" s="11">
         <v>44258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23">
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24">
+        <v>50</v>
+      </c>
+      <c r="F24">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all members sprint task assgined for sprint1
</commit_message>
<xml_diff>
--- a/Team10Report.xlsx
+++ b/Team10Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yikanwang/Documents/Spring2021/SSW555/SSW-555-A-Project-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E2F735-DAE3-524B-8763-EDE43DD85B51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55852409-AB73-3648-BE48-FD1534384843}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Burndown" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint1" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="101">
   <si>
     <t>Initials</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -353,6 +353,36 @@
   </si>
   <si>
     <t>coding</t>
+  </si>
+  <si>
+    <t>myl</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Store death date</t>
+  </si>
+  <si>
+    <t>Compare to birth date and death date</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>T06.01</t>
+  </si>
+  <si>
+    <t>Store divorce date</t>
+  </si>
+  <si>
+    <t>T06.02</t>
+  </si>
+  <si>
+    <t>T06.03</t>
+  </si>
+  <si>
+    <t>Cpmpare to divorce date and death date</t>
   </si>
 </sst>
 </file>
@@ -363,7 +393,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +427,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -419,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -440,6 +477,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1053,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7423B761-4644-4B14-9E93-F056AD5F843E}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1455,6 +1493,169 @@
         <v>50</v>
       </c>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="12">
+        <v>100</v>
+      </c>
+      <c r="F28" s="12">
+        <v>60</v>
+      </c>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="12">
+        <v>150</v>
+      </c>
+      <c r="F34" s="12">
+        <v>80</v>
+      </c>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>